<commit_message>
Minor changes in image descriptions in README.md
</commit_message>
<xml_diff>
--- a/Data/Lab 1 Experimental Data.xlsx
+++ b/Data/Lab 1 Experimental Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\FALL 2020\CSC 382\LAB 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\FALL 2020\CSC 382\LAB 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D50693A-98BF-4CC5-92A5-09B8D26F78F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC173FEE-88F7-4969-BD03-555257AB3FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7470" yWindow="5530" windowWidth="28150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fixed mistake in data set for insertion sort 50 arrays N=100 steps
</commit_message>
<xml_diff>
--- a/Data/Lab 1 Experimental Data.xlsx
+++ b/Data/Lab 1 Experimental Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\FALL 2020\CSC 382\LAB 1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC173FEE-88F7-4969-BD03-555257AB3FFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C9F8ED-C4A5-4D01-81FC-635AEEA68ADD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="5530" windowWidth="28150" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8740" yWindow="2370" windowWidth="28250" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,8 +397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,13 +818,13 @@
         <v>8262</v>
       </c>
       <c r="F21">
-        <v>7920</v>
+        <v>6232</v>
       </c>
       <c r="G21">
-        <v>6232</v>
+        <v>67632</v>
       </c>
       <c r="H21">
-        <v>67632</v>
+        <v>10507</v>
       </c>
       <c r="I21">
         <v>8264</v>

</xml_diff>